<commit_message>
Added feature to create checklists for each associate
</commit_message>
<xml_diff>
--- a/.Net Requirements.xlsx
+++ b/.Net Requirements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Revature-Capstone-1362\construct-trello-boards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE6D0483-38CE-4B41-873A-5A1356FB32A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8BA5B31-16EB-4CED-91C8-6B67EA7B2097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9900" yWindow="4275" windowWidth="23550" windowHeight="15600" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Weekly Counter" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="117">
   <si>
     <t>GitHub Repository</t>
   </si>
@@ -129,21 +129,270 @@
     <t>Week 4</t>
   </si>
   <si>
-    <t>Week 3</t>
-  </si>
-  <si>
-    <t>Week 2</t>
-  </si>
-  <si>
-    <t>Week 1</t>
+    <t>Week 1 (Project Design)</t>
+  </si>
+  <si>
+    <t>Week 2 (Data Structures)</t>
+  </si>
+  <si>
+    <t>Week 3 (Endpoints-ASP.NET)</t>
+  </si>
+  <si>
+    <t>Set up repository for Project 1</t>
+  </si>
+  <si>
+    <t>Clone to your computer and initialize</t>
+  </si>
+  <si>
+    <t>First Commit</t>
+  </si>
+  <si>
+    <t>First Push</t>
+  </si>
+  <si>
+    <t>Local Directory (Folder)</t>
+  </si>
+  <si>
+    <t>GitHub Add</t>
+  </si>
+  <si>
+    <t>GitHub Commit</t>
+  </si>
+  <si>
+    <t>GitHub Push</t>
+  </si>
+  <si>
+    <t>Make a Habit to sign all commits</t>
+  </si>
+  <si>
+    <t>Understand what your application is meant to do.</t>
+  </si>
+  <si>
+    <t>Review the architecture diagram</t>
+  </si>
+  <si>
+    <t>Draft an outline of use-cases for the project (Optional)</t>
+  </si>
+  <si>
+    <t>Initialize Project</t>
+  </si>
+  <si>
+    <t>Add Required Dependencies</t>
+  </si>
+  <si>
+    <t>User ID</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>Resolver</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Resource Not Found Exception</t>
+  </si>
+  <si>
+    <t>Username Not Available Exception</t>
+  </si>
+  <si>
+    <t>Invalid Credentials Exception</t>
+  </si>
+  <si>
+    <t>SQL Script to create tables</t>
+  </si>
+  <si>
+    <t>Insert default employee and manager users</t>
+  </si>
+  <si>
+    <t>Get Instance Method</t>
+  </si>
+  <si>
+    <t>Get Connection Method</t>
+  </si>
+  <si>
+    <t>Get User by ID Method</t>
+  </si>
+  <si>
+    <t>Get User by Username Method</t>
+  </si>
+  <si>
+    <t>Create User Method</t>
+  </si>
+  <si>
+    <t>Get All Users Method</t>
+  </si>
+  <si>
+    <t>Get Reimbursement</t>
+  </si>
+  <si>
+    <t>by ID Method</t>
+  </si>
+  <si>
+    <t>Get Reimbursements by Author Method</t>
+  </si>
+  <si>
+    <t>Get Reimbursments by Status Method</t>
+  </si>
+  <si>
+    <t>Create Reimbursement Method</t>
+  </si>
+  <si>
+    <t>Update Reimbursement Method</t>
+  </si>
+  <si>
+    <t>Register Method</t>
+  </si>
+  <si>
+    <t>Login Method</t>
+  </si>
+  <si>
+    <t>Submit Reimbursement Method</t>
+  </si>
+  <si>
+    <t>Update (Process) Reimbursement Method</t>
+  </si>
+  <si>
+    <t>Get Reimbursements by ID Method</t>
+  </si>
+  <si>
+    <t>Get All Reimbursements by UserID Method</t>
+  </si>
+  <si>
+    <t>Get Reimbursements by Status Method</t>
+  </si>
+  <si>
+    <t>Add Project Dependencies as references in API.csproj file</t>
+  </si>
+  <si>
+    <t>Register classes in dependecy injection container in program.cs file</t>
+  </si>
+  <si>
+    <t>Configure swagger api integration in program.cs file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GitHub Commit </t>
+  </si>
+  <si>
+    <t>Get all Users Handler</t>
+  </si>
+  <si>
+    <t>Get by Username Handler</t>
+  </si>
+  <si>
+    <t>Get by ID Handler</t>
+  </si>
+  <si>
+    <t>Submit Handler</t>
+  </si>
+  <si>
+    <t>Process Handler</t>
+  </si>
+  <si>
+    <t>Get by Status Handler</t>
+  </si>
+  <si>
+    <t>Get by Author Handler</t>
+  </si>
+  <si>
+    <t>Test Login Fails when Password Incorrect</t>
+  </si>
+  <si>
+    <t>Test Login Fails when Username Doesn't Exist</t>
+  </si>
+  <si>
+    <t>Test Register Fails when Username Already Exists</t>
+  </si>
+  <si>
+    <t>MapGet for /user (could have username query parameter)</t>
+  </si>
+  <si>
+    <t>MapGet for /user/{userId}</t>
+  </si>
+  <si>
+    <t>MapPost for /login</t>
+  </si>
+  <si>
+    <t>MapGet for /tickets (could have author or status query parameter)</t>
+  </si>
+  <si>
+    <t>MapPost for /submit</t>
+  </si>
+  <si>
+    <t>MapPut for /process</t>
+  </si>
+  <si>
+    <t>Make Sure it Works/Runs!</t>
+  </si>
+  <si>
+    <t>Test Through Swagger API</t>
+  </si>
+  <si>
+    <t>Prepare</t>
+  </si>
+  <si>
+    <t>Presentation</t>
+  </si>
+  <si>
+    <t>Git Hub Check List Items</t>
+  </si>
+  <si>
+    <t>Project Repository Check List Items</t>
+  </si>
+  <si>
+    <t>Signed Commits Check List Items</t>
+  </si>
+  <si>
+    <t>Use-Case Design Check List Items</t>
+  </si>
+  <si>
+    <t>Create Class Library Project for Models Check List Items</t>
+  </si>
+  <si>
+    <t>User Model Class Checklist Items</t>
+  </si>
+  <si>
+    <t>Ticket Model Class CheckList Items</t>
+  </si>
+  <si>
+    <t>Custom Exceptions CheckList Items</t>
+  </si>
+  <si>
+    <t>Week 1 Cards</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -169,8 +418,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -488,7 +738,7 @@
   <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -540,7 +790,7 @@
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
@@ -550,7 +800,7 @@
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -560,62 +810,225 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="34.28515625" customWidth="1"/>
-    <col min="2" max="2" width="38.140625" customWidth="1"/>
-    <col min="3" max="3" width="22.5703125" customWidth="1"/>
+    <col min="2" max="2" width="37.85546875" customWidth="1"/>
+    <col min="3" max="3" width="33" customWidth="1"/>
+    <col min="4" max="4" width="32.5703125" customWidth="1"/>
+    <col min="5" max="5" width="54" customWidth="1"/>
+    <col min="6" max="6" width="53.5703125" customWidth="1"/>
+    <col min="7" max="7" width="31" customWidth="1"/>
+    <col min="8" max="9" width="32.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H3" t="s">
+        <v>55</v>
+      </c>
+      <c r="I3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" t="s">
+        <v>52</v>
+      </c>
+      <c r="H4" t="s">
+        <v>56</v>
+      </c>
+      <c r="I4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H5" t="s">
+        <v>57</v>
+      </c>
+      <c r="I5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="F6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H6" t="s">
+        <v>58</v>
+      </c>
+      <c r="I6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="G7" t="s">
+        <v>42</v>
+      </c>
+      <c r="H7" t="s">
+        <v>59</v>
+      </c>
+      <c r="I7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="G8" t="s">
+        <v>43</v>
+      </c>
+      <c r="H8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>21</v>
       </c>
+      <c r="H9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -625,60 +1038,213 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{801FADF7-20D0-4EA5-9EFC-6007B8598E3F}">
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="40.28515625" customWidth="1"/>
+    <col min="2" max="2" width="28.5703125" customWidth="1"/>
+    <col min="3" max="3" width="37.28515625" customWidth="1"/>
+    <col min="4" max="4" width="35.5703125" customWidth="1"/>
+    <col min="5" max="5" width="36.85546875" customWidth="1"/>
+    <col min="6" max="6" width="35.5703125" customWidth="1"/>
+    <col min="7" max="7" width="27.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5" t="s">
+        <v>73</v>
+      </c>
+      <c r="E5" t="s">
+        <v>74</v>
+      </c>
+      <c r="F5" t="s">
+        <v>75</v>
+      </c>
+      <c r="G5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" t="s">
+        <v>42</v>
+      </c>
+      <c r="G8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>23</v>
+      </c>
+      <c r="B9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D9" t="s">
+        <v>81</v>
+      </c>
+      <c r="E9" t="s">
+        <v>82</v>
+      </c>
+      <c r="F9" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -688,50 +1254,172 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8F797CB-0263-42F0-8E0C-33DB5B29E51A}">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.7109375" customWidth="1"/>
+    <col min="2" max="2" width="49.28515625" customWidth="1"/>
+    <col min="3" max="3" width="57.28515625" customWidth="1"/>
+    <col min="4" max="4" width="44.42578125" customWidth="1"/>
+    <col min="5" max="5" width="57.5703125" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D4" t="s">
+        <v>93</v>
+      </c>
+      <c r="E4" t="s">
+        <v>94</v>
+      </c>
+      <c r="F4" t="s">
+        <v>90</v>
+      </c>
+      <c r="G4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H4" t="s">
+        <v>87</v>
+      </c>
+      <c r="I4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D5" t="s">
+        <v>97</v>
+      </c>
+      <c r="E5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C6" t="s">
+        <v>99</v>
+      </c>
+      <c r="D6" t="s">
+        <v>100</v>
+      </c>
+      <c r="E6" t="s">
+        <v>101</v>
+      </c>
+      <c r="F6" t="s">
+        <v>102</v>
+      </c>
+      <c r="G6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>104</v>
+      </c>
+      <c r="C7" t="s">
+        <v>105</v>
+      </c>
+      <c r="D7" t="s">
+        <v>106</v>
+      </c>
+      <c r="E7" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>